<commit_message>
update members in responsible_parties
</commit_message>
<xml_diff>
--- a/cmip6/responsible_parties/cmip6_cmcc_responsible_parties.xlsx
+++ b/cmip6/responsible_parties/cmip6_cmcc_responsible_parties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipsl/Engineering/esdoc/bash/cmip6/responsible_parties/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/responsible_parties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F9912-A739-AB48-BDD0-24089904ED3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D551142E-B57D-AE4A-9943-0B0E0C347836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25320" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25320" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>ES-DOC CMIP6 Model Responsible Parties</t>
   </si>
@@ -144,12 +144,147 @@
   <si>
     <t>ORCID ID</t>
   </si>
+  <si>
+    <t>PEANO-DANIELE</t>
+  </si>
+  <si>
+    <t>Daniele Peano</t>
+  </si>
+  <si>
+    <t>daniele.peano@cmcc.it</t>
+  </si>
+  <si>
+    <t>http://orcid.org/0000-0002-6975-4447</t>
+  </si>
+  <si>
+    <t>CMCC</t>
+  </si>
+  <si>
+    <t>Viale Carlo Berti Pichat, 6/2
+40127, Bologna
+Italy</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/peano-daniele</t>
+  </si>
+  <si>
+    <t>LOVATO-TOMAS</t>
+  </si>
+  <si>
+    <t>Tomas Lovato</t>
+  </si>
+  <si>
+    <t>tomas.lovato@cmcc.it</t>
+  </si>
+  <si>
+    <t>Viale Carlo Berti Pichat, 6/2
+40127, Bologna - Italy</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/lovato-tomas-2</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-5188-6767</t>
+  </si>
+  <si>
+    <t>SCOCCIMARRO-ENRICO</t>
+  </si>
+  <si>
+    <t>Enrico Scoccimarro</t>
+  </si>
+  <si>
+    <t>enrico.sccccimarro@cmcc.it</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-7987-4744</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/scoccimarro-enrico-2</t>
+  </si>
+  <si>
+    <t>GUALDI-SILVIO</t>
+  </si>
+  <si>
+    <t>Silvio Gualdi</t>
+  </si>
+  <si>
+    <t>silvio.gualdi@cmcc.it</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-7777-8935</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/gualdi-silvio</t>
+  </si>
+  <si>
+    <t>momme.butenschon@cmcc.it</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/butenschon-momme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Momme Butenschön </t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-4592-9927</t>
+  </si>
+  <si>
+    <t>Dario Nicolì</t>
+  </si>
+  <si>
+    <t>NICOLÌ-DARIO</t>
+  </si>
+  <si>
+    <t>BUTENSCHÖN-MOMME</t>
+  </si>
+  <si>
+    <t>dario.nicoli@cmcc.it</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/nicoli-dario</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-5890-9346</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/fogli-pier-giuseppe</t>
+  </si>
+  <si>
+    <t>piergiuseppe.fogli@cmcc.it</t>
+  </si>
+  <si>
+    <t>FOGLI-PIER-GIUSEPPE</t>
+  </si>
+  <si>
+    <t>Pier Giuseppe Fogli</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-7997-6273</t>
+  </si>
+  <si>
+    <t>MASINA-SIMONA</t>
+  </si>
+  <si>
+    <t>Simona Masina</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-6273-7065</t>
+  </si>
+  <si>
+    <t>https://www.cmcc.it/people/masina-simona-2</t>
+  </si>
+  <si>
+    <t>simona.masina@cmcc.it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -221,6 +356,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -248,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -402,13 +550,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -529,8 +691,33 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1691,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1800,8 +1987,8 @@
   </sheetPr>
   <dimension ref="A1:IV28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2128,10 +2315,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV30"/>
+  <dimension ref="A1:IV34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2139,8 +2326,9 @@
     <col min="1" max="1" width="25.83203125" style="36" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="36" customWidth="1"/>
     <col min="3" max="4" width="29.83203125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" style="36" customWidth="1"/>
-    <col min="6" max="7" width="26.5" style="36" customWidth="1"/>
+    <col min="5" max="5" width="25" style="36" customWidth="1"/>
+    <col min="6" max="6" width="26.5" style="36" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" style="36" customWidth="1"/>
     <col min="8" max="256" width="16.33203125" style="36" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2179,85 +2367,207 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="39" t="s">
+        <v>29</v>
+      </c>
       <c r="G3" s="39"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="40"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+    <row r="4" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="40"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="A6" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="A7" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="47" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
+      <c r="A8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="40"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
+      <c r="A9" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
+      <c r="A10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="A11" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="40"/>
@@ -2273,7 +2583,7 @@
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
     </row>
@@ -2368,40 +2678,40 @@
       <c r="G23" s="42"/>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="43"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="43"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="43"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="43"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="43"/>
@@ -2430,6 +2740,42 @@
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
     </row>
+    <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="43"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+    </row>
+    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="43"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+    </row>
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="43"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+    </row>
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="43"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>